<commit_message>
feat: Phase 6  LinkedIn Brand Engine + Hybrid Refiner
NEW FILES:
- connectors/github_monitor.py: GitHubActivityMonitor class
  (tracks new repos, commits, stars, README updates, generates post ideas)
- tools/post_scheduler.py: generate_weekly_posts + hybrid_refine
  (3 modes: local/hybrid/web_copilot, Claude web UI polishing)
- scheduler.py: Background scheduler (schedule lib, Monday 9am posts)
- setup_scheduler_windows.py: Windows Task Scheduler setup

MODIFIED:
- memory/db.py: Added github_state table
- memory/excel_logger.py: Added linkedin_posts.xlsx tracking
- agent.py: Added _try_brand routing (brand check, weekly posts, hybrid)
- chrome_extension/content_script.js: task_id passthrough for hybrid

VERIFIED:
- 3 weekly posts generated (510, 513, 493 words)
- GitHub monitor: 22 activities detected
- Excel logging: linkedin_posts.xlsx created with 4 entries
- Agent routing: brand/schedule commands work correctly
</commit_message>
<xml_diff>
--- a/memory/applied_jobs.xlsx
+++ b/memory/applied_jobs.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -620,6 +620,52 @@
       </c>
       <c r="J3" s="2" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2026-03-01</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Verify</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>99</v>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Remote</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>